<commit_message>
Issue | #293 | ajuste para la importacion de empleado
</commit_message>
<xml_diff>
--- a/public/formats/co-workers.xlsx
+++ b/public/formats/co-workers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRUEBAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cofacturador\public\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E77FCCE-EB8D-4392-BB12-F5C7174921BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A31BF-72FB-4E9A-8815-B632F2E1CFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -7270,10 +7270,10 @@
     <t xml:space="preserve"> Codigo</t>
   </si>
   <si>
-    <t>pension(n=no,s=si)</t>
-  </si>
-  <si>
-    <t>salario_integral(n=no,s=si)</t>
+    <t>pension</t>
+  </si>
+  <si>
+    <t>salario_integral</t>
   </si>
 </sst>
 </file>
@@ -7660,7 +7660,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>